<commit_message>
Updated translation & template
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egorpetryaev/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA87F99-2BAB-3D49-A4E1-66398CD35D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28880" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,70 +25,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publication Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coauthors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">НЕКОТОРЫЕ РЕЗУЛЬТАТЫ РАБОТЫ ПЕРВОГО В МИРЕ СКАНИРУЮЩЕГО ЗОНДОВОГО МИКРОСКОПА - СПУТНИКА ЗЕМЛИ В ВАКУУМЕ НА ВЫСОТАХ ОКОЛО 500 КМ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Петряев Е.О.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Логинов Б.А., Хрипунов Ю.В., Щербина М.А., Смирнов А.А., Нехаенко Н.С., Гранаткин П.А., Hedeya H.Y.H., Калназарова Н., Петряев Е.О., Tanasa C.K., Ахророва Х., Маккой А.К., Айнулова Д.Р., Плужник М.Н., Мизгайло А.А., Бобарыкина В.А., Мамикоян М.В., Измайлова А.Р.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Вакуумная техника, материалы и технология. Тезисы XVIII международной научно-технической конференции. Москва.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0F1115"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Суворов А.Л., Логинов Б.А., Макеев О.Н. "Способ и устройство контроля и исследования поверхности внутри ядерных и термоядерных установок". Патент на изобретение № RU 2169954 C1, 27.07.2000.
-Логинов Б.А. "Комплекс зондовой микроскопии для работы в космическом пространстве и атмосфере". Патент на изобретение № RU 2778278 C1, 17.08.2022.
-Логинов Б.А. "Первый в мире сканирующий зондовый микроскоп в виде спутника - как старт этапа научных спутников-лабораторий". Наноиндустрия, 2021, №5, с.22-26. EDN: BACCZI.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0F1115"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/li&gt;&lt;/ul&gt;</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Publication Year</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Coauthors</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Citations</t>
+  </si>
+  <si>
+    <t>НЕКОТОРЫЕ РЕЗУЛЬТАТЫ РАБОТЫ ПЕРВОГО В МИРЕ СКАНИРУЮЩЕГО ЗОНДОВОГО МИКРОСКОПА - СПУТНИКА ЗЕМЛИ В ВАКУУМЕ НА ВЫСОТАХ ОКОЛО 500 КМ</t>
+  </si>
+  <si>
+    <t>Петряев Е.О.</t>
+  </si>
+  <si>
+    <t>Логинов Б.А., Хрипунов Ю.В., Щербина М.А., Смирнов А.А., Нехаенко Н.С., Гранаткин П.А., Hedeya H.Y.H., Калназарова Н., Петряев Е.О., Tanasa C.K., Ахророва Х., Маккой А.К., Айнулова Д.Р., Плужник М.Н., Мизгайло А.А., Бобарыкина В.А., Мамикоян М.В., Измайлова А.Р.</t>
+  </si>
+  <si>
+    <t>Вакуумная техника, материалы и технология. Тезисы XVIII международной научно-технической конференции. Москва.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,31 +70,9 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FF0F1115"/>
       <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF0F1115"/>
-      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -130,7 +86,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -138,57 +94,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -247,60 +170,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e97132"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196b24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -332,7 +271,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -356,7 +295,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -416,36 +355,35 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="56.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="61.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="77.83"/>
+    <col min="1" max="1" width="56.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="6" width="77.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -465,11 +403,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="147" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3">
         <v>2024</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -481,17 +419,12 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
+      <c r="F2" s="3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>